<commit_message>
Classroom supporting materials ready for delivery.
</commit_message>
<xml_diff>
--- a/workshop-docs/schedule.xlsx
+++ b/workshop-docs/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22520" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="1960" windowWidth="33600" windowHeight="20560" tabRatio="500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Standard Schedule (2)" sheetId="4" state="hidden" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="121">
   <si>
     <t>9:00a</t>
   </si>
@@ -358,6 +358,36 @@
   </si>
   <si>
     <t>DynamoDB Overview</t>
+  </si>
+  <si>
+    <t>Java SDK + S3 Overview</t>
+  </si>
+  <si>
+    <t>Challenge Overview</t>
+  </si>
+  <si>
+    <t>RDS Overview</t>
+  </si>
+  <si>
+    <t>RDS, Read Replicas, and Connection Discovery</t>
+  </si>
+  <si>
+    <t>S3 for Profile Pictures</t>
+  </si>
+  <si>
+    <t>S3 Object Overview</t>
+  </si>
+  <si>
+    <t>ETS, SNS, and SQS Overview</t>
+  </si>
+  <si>
+    <t>Elastic Transcoder Service</t>
+  </si>
+  <si>
+    <t>CloudWatch Overview</t>
+  </si>
+  <si>
+    <t>Emit Custom CloudWatch Metrics</t>
   </si>
 </sst>
 </file>
@@ -654,7 +684,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="455">
+  <cellStyleXfs count="473">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1110,8 +1140,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1195,39 +1243,78 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1236,36 +1323,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1315,22 +1372,40 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1339,44 +1414,41 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="455">
+  <cellStyles count="473">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1604,6 +1676,15 @@
     <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1831,6 +1912,15 @@
     <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2205,7 +2295,7 @@
       <c r="F2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="36" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2213,25 +2303,25 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="51"/>
+      <c r="H3" s="37"/>
     </row>
     <row r="4" spans="1:8" ht="29" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="F4" s="53"/>
-      <c r="H4" s="54" t="s">
+      <c r="B4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="F4" s="42"/>
+      <c r="H4" s="43" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2239,23 +2329,23 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="F5" s="41" t="s">
+      <c r="B5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="F5" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="54"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8" ht="29" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="D6" s="35" t="s">
+      <c r="B6" s="39"/>
+      <c r="D6" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="H6" s="55" t="s">
+      <c r="F6" s="45"/>
+      <c r="H6" s="47" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2263,21 +2353,21 @@
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="D7" s="37"/>
-      <c r="F7" s="42"/>
-      <c r="H7" s="55"/>
+      <c r="B7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="F7" s="45"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:8" ht="29" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="39"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="H8" s="56" t="s">
+      <c r="F8" s="46"/>
+      <c r="H8" s="48" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2285,14 +2375,14 @@
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="D9" s="35" t="s">
+      <c r="B9" s="40"/>
+      <c r="D9" s="38" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:8" ht="29" customHeight="1">
       <c r="A10" s="3" t="s">
@@ -2301,8 +2391,8 @@
       <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="F10" s="41" t="s">
+      <c r="D10" s="39"/>
+      <c r="F10" s="44" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2313,40 +2403,40 @@
       <c r="B11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="F11" s="42"/>
+      <c r="D11" s="39"/>
+      <c r="F11" s="45"/>
     </row>
     <row r="12" spans="1:8" ht="29" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="F12" s="42"/>
+      <c r="D12" s="39"/>
+      <c r="F12" s="45"/>
     </row>
     <row r="13" spans="1:8" ht="29" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="40"/>
       <c r="D13" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="43"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:8" ht="29" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="49" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2354,29 +2444,29 @@
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="F15" s="48"/>
+      <c r="B15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:8" ht="29" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="F16" s="49"/>
+      <c r="B16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" ht="29" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="57" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2384,19 +2474,19 @@
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="D18" s="45"/>
-      <c r="F18" s="46"/>
+      <c r="B18" s="40"/>
+      <c r="D18" s="58"/>
+      <c r="F18" s="59"/>
     </row>
     <row r="19" spans="1:6" ht="29" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="F19" s="35" t="s">
+      <c r="D19" s="58"/>
+      <c r="F19" s="38" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2404,11 +2494,11 @@
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="53"/>
       <c r="D20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="36"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6" ht="29" customHeight="1">
       <c r="A21" s="3" t="s">
@@ -2417,25 +2507,25 @@
       <c r="B21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="36"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:6" ht="29" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="17"/>
-      <c r="D22" s="36"/>
-      <c r="F22" s="37"/>
+      <c r="D22" s="39"/>
+      <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6" ht="29" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="18"/>
-      <c r="D23" s="36"/>
+      <c r="D23" s="39"/>
       <c r="F23" s="8" t="s">
         <v>35</v>
       </c>
@@ -2444,11 +2534,11 @@
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="F24" s="41" t="s">
+      <c r="D24" s="39"/>
+      <c r="F24" s="44" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2456,29 +2546,29 @@
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="D25" s="37"/>
-      <c r="F25" s="42"/>
+      <c r="B25" s="45"/>
+      <c r="D25" s="40"/>
+      <c r="F25" s="45"/>
     </row>
     <row r="26" spans="1:6" ht="29" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="42"/>
+      <c r="B26" s="45"/>
       <c r="D26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="42"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:6" ht="29" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="D27" s="38" t="s">
+      <c r="B27" s="46"/>
+      <c r="D27" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="43"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="1:6" ht="29" customHeight="1">
       <c r="A28" s="3" t="s">
@@ -2487,7 +2577,7 @@
       <c r="B28" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="39"/>
+      <c r="D28" s="56"/>
       <c r="F28" s="8" t="s">
         <v>35</v>
       </c>
@@ -2496,11 +2586,11 @@
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="39"/>
-      <c r="F29" s="35" t="s">
+      <c r="D29" s="56"/>
+      <c r="F29" s="38" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2508,35 +2598,35 @@
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="D30" s="39"/>
-      <c r="F30" s="36"/>
+      <c r="B30" s="55"/>
+      <c r="D30" s="56"/>
+      <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:6" ht="29" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="39"/>
-      <c r="F31" s="36"/>
+      <c r="D31" s="56"/>
+      <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:6" ht="29" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="D32" s="39"/>
-      <c r="F32" s="36"/>
+      <c r="B32" s="39"/>
+      <c r="D32" s="56"/>
+      <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6" ht="29" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="D33" s="40"/>
-      <c r="F33" s="37"/>
+      <c r="B33" s="40"/>
+      <c r="D33" s="53"/>
+      <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6" ht="29" customHeight="1">
       <c r="A34" s="3" t="s">
@@ -2569,6 +2659,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="F3:F4"/>
@@ -2581,21 +2686,6 @@
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="F10:F13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F29:F33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="F17:F18"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2655,7 +2745,7 @@
       <c r="F2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="36" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2663,25 +2753,25 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="51"/>
+      <c r="H3" s="37"/>
     </row>
     <row r="4" spans="1:8" ht="29" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="D4" s="42"/>
-      <c r="F4" s="53"/>
-      <c r="H4" s="54" t="s">
+      <c r="B4" s="39"/>
+      <c r="D4" s="45"/>
+      <c r="F4" s="42"/>
+      <c r="H4" s="43" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2689,21 +2779,21 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="D5" s="42"/>
-      <c r="F5" s="41" t="s">
+      <c r="B5" s="39"/>
+      <c r="D5" s="45"/>
+      <c r="F5" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="54"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8" ht="29" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="D6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="H6" s="55" t="s">
+      <c r="B6" s="39"/>
+      <c r="D6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="H6" s="47" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2711,21 +2801,21 @@
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="D7" s="43"/>
-      <c r="F7" s="42"/>
-      <c r="H7" s="55"/>
+      <c r="B7" s="39"/>
+      <c r="D7" s="46"/>
+      <c r="F7" s="45"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:8" ht="29" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="39"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="H8" s="56" t="s">
+      <c r="F8" s="46"/>
+      <c r="H8" s="48" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2733,14 +2823,14 @@
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="D9" s="35" t="s">
+      <c r="B9" s="40"/>
+      <c r="D9" s="38" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:8" ht="29" customHeight="1">
       <c r="A10" s="3" t="s">
@@ -2749,8 +2839,8 @@
       <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="F10" s="41" t="s">
+      <c r="D10" s="39"/>
+      <c r="F10" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2758,19 +2848,19 @@
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="F11" s="42"/>
+      <c r="D11" s="39"/>
+      <c r="F11" s="45"/>
     </row>
     <row r="12" spans="1:8" ht="29" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="D12" s="36"/>
-      <c r="F12" s="42"/>
+      <c r="B12" s="61"/>
+      <c r="D12" s="39"/>
+      <c r="F12" s="45"/>
     </row>
     <row r="13" spans="1:8" ht="29" customHeight="1">
       <c r="A13" s="3" t="s">
@@ -2779,20 +2869,20 @@
       <c r="B13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="F13" s="43"/>
+      <c r="D13" s="40"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:8" ht="29" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="49" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2800,29 +2890,29 @@
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="F15" s="48"/>
+      <c r="B15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:8" ht="29" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="F16" s="49"/>
+      <c r="B16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" ht="29" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="52" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="54" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2830,19 +2920,19 @@
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="D18" s="44" t="s">
+      <c r="B18" s="56"/>
+      <c r="D18" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="34"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:6" ht="29" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="D19" s="45"/>
-      <c r="F19" s="35" t="s">
+      <c r="B19" s="56"/>
+      <c r="D19" s="58"/>
+      <c r="F19" s="38" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2850,9 +2940,9 @@
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="D20" s="45"/>
-      <c r="F20" s="36"/>
+      <c r="B20" s="53"/>
+      <c r="D20" s="58"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6" ht="29" customHeight="1">
       <c r="A21" s="3" t="s">
@@ -2861,27 +2951,27 @@
       <c r="B21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="46"/>
-      <c r="F21" s="36"/>
+      <c r="D21" s="59"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:6" ht="29" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="38" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6" ht="29" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="D23" s="35" t="s">
+      <c r="B23" s="39"/>
+      <c r="D23" s="38" t="s">
         <v>43</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -2892,9 +2982,9 @@
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="F24" s="41" t="s">
+      <c r="B24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="F24" s="44" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2902,9 +2992,9 @@
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="D25" s="36"/>
-      <c r="F25" s="42"/>
+      <c r="B25" s="40"/>
+      <c r="D25" s="39"/>
+      <c r="F25" s="45"/>
     </row>
     <row r="26" spans="1:6" ht="29" customHeight="1">
       <c r="A26" s="3" t="s">
@@ -2913,24 +3003,24 @@
       <c r="B26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="F26" s="42"/>
+      <c r="D26" s="39"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:6" ht="29" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="F27" s="43"/>
+      <c r="D27" s="40"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="1:6" ht="29" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="36"/>
+      <c r="B28" s="39"/>
       <c r="D28" s="8" t="s">
         <v>35</v>
       </c>
@@ -2942,11 +3032,11 @@
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="D29" s="38" t="s">
+      <c r="B29" s="39"/>
+      <c r="D29" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="38" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2954,33 +3044,33 @@
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="D30" s="39"/>
-      <c r="F30" s="36"/>
+      <c r="B30" s="39"/>
+      <c r="D30" s="56"/>
+      <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:6" ht="29" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="D31" s="39"/>
-      <c r="F31" s="36"/>
+      <c r="B31" s="39"/>
+      <c r="D31" s="56"/>
+      <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:6" ht="29" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="D32" s="39"/>
-      <c r="F32" s="36"/>
+      <c r="B32" s="39"/>
+      <c r="D32" s="56"/>
+      <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6" ht="29" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="D33" s="40"/>
-      <c r="F33" s="37"/>
+      <c r="B33" s="40"/>
+      <c r="D33" s="53"/>
+      <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6" ht="29" customHeight="1">
       <c r="A34" s="3" t="s">
@@ -2996,6 +3086,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="B27:B33"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H6:H7"/>
@@ -3008,18 +3110,6 @@
     <mergeCell ref="F5:F8"/>
     <mergeCell ref="F10:F13"/>
     <mergeCell ref="F14:F16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="B27:B33"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3079,7 +3169,7 @@
       <c r="F2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="36" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3087,25 +3177,25 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="51"/>
+      <c r="H3" s="37"/>
     </row>
     <row r="4" spans="1:12" ht="29" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="D4" s="42"/>
-      <c r="F4" s="53"/>
-      <c r="H4" s="54" t="s">
+      <c r="B4" s="39"/>
+      <c r="D4" s="45"/>
+      <c r="F4" s="42"/>
+      <c r="H4" s="43" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3113,21 +3203,21 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="D5" s="42"/>
-      <c r="F5" s="41" t="s">
+      <c r="B5" s="39"/>
+      <c r="D5" s="45"/>
+      <c r="F5" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="54"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:12" ht="29" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="D6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="H6" s="55" t="s">
+      <c r="B6" s="39"/>
+      <c r="D6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="H6" s="47" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3135,21 +3225,21 @@
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="D7" s="43"/>
-      <c r="F7" s="42"/>
-      <c r="H7" s="55"/>
+      <c r="B7" s="39"/>
+      <c r="D7" s="46"/>
+      <c r="F7" s="45"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:12" ht="29" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="39"/>
       <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="H8" s="56" t="s">
+      <c r="F8" s="46"/>
+      <c r="H8" s="48" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3157,14 +3247,14 @@
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="D9" s="35" t="s">
+      <c r="B9" s="40"/>
+      <c r="D9" s="38" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:12" ht="29" customHeight="1">
       <c r="A10" s="3" t="s">
@@ -3173,8 +3263,8 @@
       <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="F10" s="41" t="s">
+      <c r="D10" s="39"/>
+      <c r="F10" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3185,41 +3275,41 @@
       <c r="B11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="F11" s="42"/>
+      <c r="D11" s="39"/>
+      <c r="F11" s="45"/>
     </row>
     <row r="12" spans="1:12" ht="29" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="F12" s="42"/>
+      <c r="D12" s="39"/>
+      <c r="F12" s="45"/>
     </row>
     <row r="13" spans="1:12" ht="29" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="F13" s="43"/>
+      <c r="B13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:12" ht="29" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="62" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3227,19 +3317,19 @@
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="L15" s="60"/>
+      <c r="B15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="L15" s="63"/>
     </row>
     <row r="16" spans="1:12" ht="29" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="L16" s="61"/>
+      <c r="B16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="L16" s="64"/>
     </row>
     <row r="17" spans="1:12" ht="29" customHeight="1">
       <c r="A17" s="3" t="s">
@@ -3251,7 +3341,7 @@
       <c r="D17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="54" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3259,24 +3349,24 @@
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="34"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:12" ht="29" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="D19" s="45"/>
-      <c r="F19" s="35" t="s">
+      <c r="B19" s="56"/>
+      <c r="D19" s="58"/>
+      <c r="F19" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="62" t="s">
+      <c r="L19" s="65" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3284,10 +3374,10 @@
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="D20" s="46"/>
-      <c r="F20" s="36"/>
-      <c r="L20" s="63"/>
+      <c r="B20" s="53"/>
+      <c r="D20" s="59"/>
+      <c r="F20" s="39"/>
+      <c r="L20" s="66"/>
     </row>
     <row r="21" spans="1:12" ht="29" customHeight="1">
       <c r="A21" s="3" t="s">
@@ -3296,8 +3386,8 @@
       <c r="B21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="36"/>
-      <c r="L21" s="63"/>
+      <c r="F21" s="39"/>
+      <c r="L21" s="66"/>
     </row>
     <row r="22" spans="1:12" ht="29" customHeight="1">
       <c r="A22" s="3" t="s">
@@ -3306,14 +3396,14 @@
       <c r="B22" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="L22" s="64"/>
+      <c r="F22" s="40"/>
+      <c r="L22" s="67"/>
     </row>
     <row r="23" spans="1:12" ht="29" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="65" t="s">
         <v>59</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -3324,8 +3414,8 @@
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="F24" s="41" t="s">
+      <c r="B24" s="66"/>
+      <c r="F24" s="44" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3333,31 +3423,31 @@
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="64"/>
+      <c r="B25" s="67"/>
       <c r="D25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="42"/>
+      <c r="F25" s="45"/>
     </row>
     <row r="26" spans="1:12" ht="29" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="42"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:12" ht="29" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="D27" s="36"/>
-      <c r="F27" s="43"/>
+      <c r="B27" s="67"/>
+      <c r="D27" s="39"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="1:12" ht="29" customHeight="1">
       <c r="A28" s="3" t="s">
@@ -3366,7 +3456,7 @@
       <c r="B28" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="36"/>
+      <c r="D28" s="39"/>
       <c r="F28" s="8" t="s">
         <v>35</v>
       </c>
@@ -3375,11 +3465,11 @@
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="F29" s="35" t="s">
+      <c r="D29" s="40"/>
+      <c r="F29" s="38" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3387,37 +3477,37 @@
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36"/>
+      <c r="B30" s="39"/>
       <c r="D30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="36"/>
+      <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:12" ht="29" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="D31" s="38" t="s">
+      <c r="B31" s="39"/>
+      <c r="D31" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="36"/>
+      <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:12" ht="29" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="D32" s="39"/>
-      <c r="F32" s="36"/>
+      <c r="B32" s="39"/>
+      <c r="D32" s="56"/>
+      <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6" ht="29" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="D33" s="40"/>
-      <c r="F33" s="37"/>
+      <c r="B33" s="40"/>
+      <c r="D33" s="53"/>
+      <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6" ht="29" customHeight="1">
       <c r="A34" s="3" t="s">
@@ -3433,17 +3523,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="F14:F16"/>
@@ -3460,6 +3539,17 @@
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="F19:F22"/>
     <mergeCell ref="L19:L22"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3521,10 +3611,10 @@
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="36" t="s">
         <v>51</v>
       </c>
       <c r="F4" s="1"/>
@@ -3536,8 +3626,8 @@
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="37"/>
       <c r="F5" s="1"/>
       <c r="H5"/>
       <c r="N5" s="1"/>
@@ -3547,10 +3637,10 @@
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="43" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="1"/>
@@ -3562,8 +3652,8 @@
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="54"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="43"/>
       <c r="F7" s="1"/>
       <c r="H7"/>
       <c r="N7" s="1"/>
@@ -3576,7 +3666,7 @@
       <c r="B8" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="47" t="s">
         <v>79</v>
       </c>
       <c r="F8" s="1"/>
@@ -3591,7 +3681,7 @@
       <c r="B9" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="55"/>
+      <c r="C9" s="47"/>
       <c r="F9" s="1"/>
       <c r="G9"/>
       <c r="N9" s="1"/>
@@ -3604,7 +3694,7 @@
       <c r="B10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="48" t="s">
         <v>86</v>
       </c>
       <c r="F10" s="1"/>
@@ -3616,10 +3706,10 @@
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="56"/>
+      <c r="C11" s="48"/>
       <c r="F11" s="1"/>
       <c r="H11"/>
       <c r="K11" s="11"/>
@@ -3630,7 +3720,7 @@
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="66"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12"/>
@@ -3642,7 +3732,7 @@
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="67"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13"/>
@@ -3654,7 +3744,7 @@
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="71" t="s">
         <v>88</v>
       </c>
       <c r="C14" s="1"/>
@@ -3668,7 +3758,7 @@
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="69"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="1"/>
       <c r="F15" s="1"/>
       <c r="N15" s="1"/>
@@ -3678,7 +3768,7 @@
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="73" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="1"/>
@@ -3690,7 +3780,7 @@
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="71"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="1"/>
       <c r="F17" s="1"/>
       <c r="N17" s="1"/>
@@ -3700,7 +3790,7 @@
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="71"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="1"/>
       <c r="F18" s="1"/>
       <c r="N18" s="1"/>
@@ -3710,7 +3800,7 @@
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="72"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="1"/>
       <c r="F19" s="1"/>
       <c r="N19" s="1"/>
@@ -3732,7 +3822,7 @@
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="68" t="s">
         <v>91</v>
       </c>
       <c r="C21" s="1"/>
@@ -3744,7 +3834,7 @@
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="66"/>
+      <c r="B22" s="69"/>
       <c r="C22" s="1"/>
       <c r="F22" s="1"/>
       <c r="N22" s="1"/>
@@ -3754,7 +3844,7 @@
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="66"/>
+      <c r="B23" s="69"/>
       <c r="F23" s="1"/>
       <c r="G23"/>
       <c r="J23" s="11"/>
@@ -3765,7 +3855,7 @@
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="67"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="1"/>
       <c r="I24"/>
       <c r="N24" s="1"/>
@@ -3787,7 +3877,7 @@
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="65" t="s">
+      <c r="B26" s="68" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="1"/>
@@ -3799,7 +3889,7 @@
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="67"/>
+      <c r="B27" s="70"/>
       <c r="C27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27"/>
@@ -3838,7 +3928,7 @@
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="65" t="s">
+      <c r="B30" s="68" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="1"/>
@@ -3852,7 +3942,7 @@
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="66"/>
+      <c r="B31" s="69"/>
       <c r="C31" s="1"/>
       <c r="F31" s="1"/>
       <c r="H31"/>
@@ -3864,7 +3954,7 @@
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="67"/>
+      <c r="B32" s="70"/>
       <c r="C32" s="1"/>
       <c r="F32" s="1"/>
       <c r="H32"/>
@@ -3888,7 +3978,7 @@
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="68" t="s">
         <v>94</v>
       </c>
       <c r="C34" s="1"/>
@@ -3900,7 +3990,7 @@
       <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="67"/>
+      <c r="B35" s="70"/>
       <c r="C35" s="1"/>
       <c r="F35" s="1"/>
       <c r="N35" s="1"/>
@@ -4011,7 +4101,7 @@
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="73" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -4026,7 +4116,7 @@
       <c r="H4" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="50" t="s">
+      <c r="J4" s="36" t="s">
         <v>51</v>
       </c>
       <c r="R4" s="1"/>
@@ -4035,38 +4125,38 @@
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="72"/>
+      <c r="B5" s="75"/>
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="78" t="s">
         <v>74</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="77" t="s">
+      <c r="H5" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="J5" s="51"/>
+      <c r="J5" s="37"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" ht="29" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="76" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="78"/>
+      <c r="E6" s="80"/>
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="78"/>
-      <c r="J6" s="54" t="s">
+      <c r="H6" s="80"/>
+      <c r="J6" s="43" t="s">
         <v>49</v>
       </c>
       <c r="R6" s="1"/>
@@ -4075,34 +4165,34 @@
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="83"/>
+      <c r="B7" s="77"/>
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="78"/>
+      <c r="E7" s="80"/>
       <c r="G7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="78"/>
-      <c r="J7" s="54"/>
+      <c r="H7" s="80"/>
+      <c r="J7" s="43"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" ht="29" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="78" t="s">
         <v>69</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="78"/>
+      <c r="E8" s="80"/>
       <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="78"/>
-      <c r="J8" s="55" t="s">
+      <c r="H8" s="80"/>
+      <c r="J8" s="47" t="s">
         <v>79</v>
       </c>
       <c r="R8" s="1"/>
@@ -4111,18 +4201,18 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="84"/>
+      <c r="B9" s="79"/>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="84"/>
+      <c r="E9" s="79"/>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="55"/>
+      <c r="J9" s="47"/>
       <c r="N9"/>
       <c r="O9" s="1"/>
       <c r="R9" s="1"/>
@@ -4143,10 +4233,10 @@
       <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="48" t="s">
         <v>65</v>
       </c>
       <c r="R10" s="1"/>
@@ -4155,34 +4245,34 @@
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="78" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="81" t="s">
+      <c r="E11" s="76" t="s">
         <v>73</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="J11" s="56"/>
+      <c r="H11" s="86"/>
+      <c r="J11" s="48"/>
     </row>
     <row r="12" spans="1:18" ht="29" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="80"/>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="82"/>
+      <c r="E12" s="81"/>
       <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="74"/>
+      <c r="H12" s="86"/>
       <c r="N12"/>
       <c r="O12" s="1"/>
       <c r="Q12" s="11"/>
@@ -4192,15 +4282,15 @@
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="80"/>
       <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="82"/>
+      <c r="E13" s="81"/>
       <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="74"/>
+      <c r="H13" s="86"/>
       <c r="N13"/>
       <c r="O13" s="1"/>
       <c r="Q13" s="11"/>
@@ -4210,15 +4300,15 @@
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="80"/>
       <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="82"/>
+      <c r="E14" s="81"/>
       <c r="G14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="75" t="s">
+      <c r="H14" s="82" t="s">
         <v>71</v>
       </c>
       <c r="N14"/>
@@ -4236,11 +4326,11 @@
       <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="83"/>
+      <c r="E15" s="77"/>
       <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="76"/>
+      <c r="H15" s="84"/>
       <c r="O15" s="1"/>
       <c r="R15" s="1"/>
     </row>
@@ -4248,19 +4338,19 @@
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="73" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="73" t="s">
         <v>38</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="70" t="s">
+      <c r="H16" s="73" t="s">
         <v>38</v>
       </c>
       <c r="O16" s="1"/>
@@ -4270,15 +4360,15 @@
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="71"/>
+      <c r="B17" s="74"/>
       <c r="D17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="71"/>
+      <c r="E17" s="74"/>
       <c r="G17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="71"/>
+      <c r="H17" s="74"/>
       <c r="O17" s="1"/>
       <c r="R17" s="1"/>
     </row>
@@ -4286,15 +4376,15 @@
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="71"/>
+      <c r="B18" s="74"/>
       <c r="D18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="71"/>
+      <c r="E18" s="74"/>
       <c r="G18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="71"/>
+      <c r="H18" s="74"/>
       <c r="O18" s="1"/>
       <c r="R18" s="1"/>
     </row>
@@ -4302,17 +4392,17 @@
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="72"/>
+      <c r="B19" s="75"/>
       <c r="D19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="72"/>
+      <c r="E19" s="75"/>
       <c r="G19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="72"/>
+      <c r="H19" s="75"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="75" t="s">
+      <c r="P19" s="82" t="s">
         <v>78</v>
       </c>
       <c r="R19" s="1"/>
@@ -4321,86 +4411,86 @@
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="78" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="75" t="s">
+      <c r="E20" s="82" t="s">
         <v>70</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="75" t="s">
+      <c r="H20" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="J20" s="81" t="s">
+      <c r="J20" s="76" t="s">
         <v>39</v>
       </c>
       <c r="O20" s="1"/>
-      <c r="P20" s="85"/>
+      <c r="P20" s="83"/>
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" ht="29" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="78"/>
+      <c r="B21" s="80"/>
       <c r="D21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="85"/>
+      <c r="E21" s="83"/>
       <c r="G21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="85"/>
-      <c r="J21" s="82"/>
+      <c r="H21" s="83"/>
+      <c r="J21" s="81"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="85"/>
+      <c r="P21" s="83"/>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" ht="29" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="84"/>
+      <c r="B22" s="79"/>
       <c r="D22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="85"/>
+      <c r="E22" s="83"/>
       <c r="G22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="76"/>
+      <c r="H22" s="84"/>
       <c r="J22" s="22" t="s">
         <v>35</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="85"/>
+      <c r="P22" s="83"/>
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" ht="29" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="88" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="85"/>
+      <c r="E23" s="83"/>
       <c r="G23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="81" t="s">
+      <c r="H23" s="76" t="s">
         <v>43</v>
       </c>
       <c r="N23"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="85"/>
+      <c r="P23" s="83"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="1"/>
     </row>
@@ -4408,18 +4498,18 @@
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="80"/>
+      <c r="B24" s="89"/>
       <c r="D24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="76"/>
+      <c r="E24" s="84"/>
       <c r="G24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="82"/>
+      <c r="H24" s="81"/>
       <c r="N24"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="76"/>
+      <c r="P24" s="84"/>
       <c r="Q24"/>
       <c r="R24" s="1"/>
     </row>
@@ -4436,7 +4526,7 @@
       <c r="G25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="82"/>
+      <c r="H25" s="81"/>
       <c r="N25"/>
       <c r="O25" s="1"/>
       <c r="Q25"/>
@@ -4449,13 +4539,13 @@
       <c r="D26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="77" t="s">
+      <c r="E26" s="78" t="s">
         <v>48</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H26" s="82"/>
+      <c r="H26" s="81"/>
       <c r="M26"/>
       <c r="O26" s="1"/>
       <c r="P26"/>
@@ -4468,7 +4558,7 @@
       <c r="D27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="78"/>
+      <c r="E27" s="80"/>
       <c r="G27" s="3" t="s">
         <v>24</v>
       </c>
@@ -4486,11 +4576,11 @@
       <c r="D28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="78"/>
+      <c r="E28" s="80"/>
       <c r="G28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="81" t="s">
+      <c r="H28" s="76" t="s">
         <v>75</v>
       </c>
       <c r="N28"/>
@@ -4505,11 +4595,11 @@
       <c r="D29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="84"/>
+      <c r="E29" s="79"/>
       <c r="G29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="82"/>
+      <c r="H29" s="81"/>
       <c r="N29"/>
       <c r="O29" s="1"/>
       <c r="Q29" s="11"/>
@@ -4528,7 +4618,7 @@
       <c r="G30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H30" s="82"/>
+      <c r="H30" s="81"/>
       <c r="N30"/>
       <c r="O30" s="1"/>
       <c r="Q30" s="11"/>
@@ -4541,29 +4631,29 @@
       <c r="D31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="73" t="s">
+      <c r="E31" s="85" t="s">
         <v>77</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="83"/>
+      <c r="H31" s="77"/>
     </row>
     <row r="32" spans="1:18" ht="29" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="77" t="s">
+      <c r="B32" s="78" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="74"/>
+      <c r="E32" s="86"/>
       <c r="G32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="77" t="s">
+      <c r="H32" s="78" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4571,15 +4661,15 @@
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="78"/>
+      <c r="B33" s="80"/>
       <c r="D33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="74"/>
+      <c r="E33" s="86"/>
       <c r="G33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="78"/>
+      <c r="H33" s="80"/>
       <c r="O33" s="1"/>
       <c r="R33" s="1"/>
     </row>
@@ -4587,15 +4677,15 @@
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="78"/>
+      <c r="B34" s="80"/>
       <c r="D34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="74"/>
+      <c r="E34" s="86"/>
       <c r="G34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="78"/>
+      <c r="H34" s="80"/>
       <c r="O34" s="1"/>
       <c r="R34" s="1"/>
     </row>
@@ -4603,15 +4693,15 @@
       <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="84"/>
+      <c r="B35" s="79"/>
       <c r="D35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="86"/>
+      <c r="E35" s="87"/>
       <c r="G35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="84"/>
+      <c r="H35" s="79"/>
       <c r="O35" s="1"/>
       <c r="R35" s="1"/>
     </row>
@@ -4636,14 +4726,14 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="E5:E9"/>
-    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="E11:E15"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="E16:E19"/>
     <mergeCell ref="H28:H31"/>
@@ -4656,14 +4746,14 @@
     <mergeCell ref="H23:H26"/>
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="H20:H22"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="E5:E9"/>
+    <mergeCell ref="H5:H8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="39" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4677,10 +4767,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4693,7 +4786,7 @@
       <c r="A2" s="32">
         <v>0.375</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="33" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4701,7 +4794,7 @@
       <c r="A3" s="32">
         <v>0.37847222222222227</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="34" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4709,7 +4802,7 @@
       <c r="A4" s="32">
         <v>0.38194444444444442</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="93" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4717,25 +4810,25 @@
       <c r="A5" s="32">
         <v>0.38541666666666669</v>
       </c>
-      <c r="B5" s="89"/>
+      <c r="B5" s="93"/>
     </row>
     <row r="6" spans="1:2" ht="11" customHeight="1">
       <c r="A6" s="32">
         <v>0.38888888888888901</v>
       </c>
-      <c r="B6" s="89"/>
+      <c r="B6" s="93"/>
     </row>
     <row r="7" spans="1:2" ht="11" customHeight="1">
       <c r="A7" s="32">
         <v>0.39236111111111099</v>
       </c>
-      <c r="B7" s="89"/>
+      <c r="B7" s="93"/>
     </row>
     <row r="8" spans="1:2" ht="11" customHeight="1">
       <c r="A8" s="32">
         <v>0.39583333333333398</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="93" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4743,7 +4836,7 @@
       <c r="A9" s="32">
         <v>0.39930555555555602</v>
       </c>
-      <c r="B9" s="89"/>
+      <c r="B9" s="93"/>
     </row>
     <row r="10" spans="1:2" ht="11" customHeight="1">
       <c r="A10" s="32">
@@ -4763,7 +4856,7 @@
       <c r="A12" s="32">
         <v>0.40972222222222299</v>
       </c>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="34" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4771,7 +4864,7 @@
       <c r="A13" s="32">
         <v>0.41319444444444497</v>
       </c>
-      <c r="B13" s="88" t="s">
+      <c r="B13" s="34" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4779,7 +4872,7 @@
       <c r="A14" s="32">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B14" s="88" t="s">
+      <c r="B14" s="34" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4787,7 +4880,7 @@
       <c r="A15" s="32">
         <v>0.42013888888889001</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="93" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4795,13 +4888,13 @@
       <c r="A16" s="32">
         <v>0.42361111111111199</v>
       </c>
-      <c r="B16" s="89"/>
+      <c r="B16" s="93"/>
     </row>
     <row r="17" spans="1:2" ht="11" customHeight="1">
       <c r="A17" s="32">
         <v>0.42708333333333398</v>
       </c>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="93" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4809,19 +4902,19 @@
       <c r="A18" s="32">
         <v>0.43055555555555602</v>
       </c>
-      <c r="B18" s="89"/>
+      <c r="B18" s="93"/>
     </row>
     <row r="19" spans="1:2" ht="11" customHeight="1">
       <c r="A19" s="32">
         <v>0.43402777777777901</v>
       </c>
-      <c r="B19" s="89"/>
+      <c r="B19" s="93"/>
     </row>
     <row r="20" spans="1:2" ht="11" customHeight="1">
       <c r="A20" s="32">
         <v>0.437500000000001</v>
       </c>
-      <c r="B20" s="91" t="s">
+      <c r="B20" s="92" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4829,13 +4922,13 @@
       <c r="A21" s="32">
         <v>0.44097222222222299</v>
       </c>
-      <c r="B21" s="91"/>
+      <c r="B21" s="92"/>
     </row>
     <row r="22" spans="1:2" ht="11" customHeight="1">
       <c r="A22" s="32">
         <v>0.44444444444444497</v>
       </c>
-      <c r="B22" s="91"/>
+      <c r="B22" s="92"/>
     </row>
     <row r="23" spans="1:2" ht="11" customHeight="1">
       <c r="A23" s="32">
@@ -4883,7 +4976,7 @@
       <c r="A29" s="32">
         <v>0.468750000000001</v>
       </c>
-      <c r="B29" s="90" t="s">
+      <c r="B29" s="98" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4891,21 +4984,25 @@
       <c r="A30" s="32">
         <v>0.47222222222222299</v>
       </c>
-      <c r="B30" s="90"/>
+      <c r="B30" s="35" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" spans="1:2" ht="11" customHeight="1">
       <c r="A31" s="32">
         <v>0.47569444444444597</v>
       </c>
-      <c r="B31" s="89" t="s">
-        <v>55</v>
+      <c r="B31" s="35" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="11" customHeight="1">
       <c r="A32" s="32">
         <v>0.47916666666666802</v>
       </c>
-      <c r="B32" s="89"/>
+      <c r="B32" s="35" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="33" spans="1:2" ht="11" customHeight="1">
       <c r="A33" s="32">
@@ -4937,7 +5034,7 @@
       <c r="A37" s="32">
         <v>0.49652777777777901</v>
       </c>
-      <c r="B37" s="87" t="s">
+      <c r="B37" s="33" t="s">
         <v>110</v>
       </c>
     </row>
@@ -4953,37 +5050,37 @@
       <c r="A39" s="32">
         <v>0.50347222222222399</v>
       </c>
-      <c r="B39" s="92"/>
+      <c r="B39" s="91"/>
     </row>
     <row r="40" spans="1:2" ht="11" customHeight="1">
       <c r="A40" s="32">
         <v>0.50694444444444597</v>
       </c>
-      <c r="B40" s="92"/>
+      <c r="B40" s="91"/>
     </row>
     <row r="41" spans="1:2" ht="11" customHeight="1">
       <c r="A41" s="32">
         <v>0.51041666666666796</v>
       </c>
-      <c r="B41" s="92"/>
+      <c r="B41" s="91"/>
     </row>
     <row r="42" spans="1:2" ht="11" customHeight="1">
       <c r="A42" s="32">
         <v>0.51388888888889095</v>
       </c>
-      <c r="B42" s="92"/>
+      <c r="B42" s="91"/>
     </row>
     <row r="43" spans="1:2" ht="11" customHeight="1">
       <c r="A43" s="32">
         <v>0.51736111111111305</v>
       </c>
-      <c r="B43" s="92"/>
+      <c r="B43" s="91"/>
     </row>
     <row r="44" spans="1:2" ht="11" customHeight="1">
       <c r="A44" s="32">
         <v>0.52083333333333504</v>
       </c>
-      <c r="B44" s="91" t="s">
+      <c r="B44" s="92" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4991,308 +5088,389 @@
       <c r="A45" s="32">
         <v>0.52430555555555702</v>
       </c>
-      <c r="B45" s="91"/>
+      <c r="B45" s="92"/>
     </row>
     <row r="46" spans="1:2" ht="11" customHeight="1">
       <c r="A46" s="32">
         <v>0.52777777777778001</v>
       </c>
-      <c r="B46" s="91"/>
+      <c r="B46" s="92"/>
     </row>
     <row r="47" spans="1:2" ht="11" customHeight="1">
       <c r="A47" s="32">
         <v>0.531250000000002</v>
       </c>
-      <c r="B47" s="91"/>
+      <c r="B47" s="92"/>
     </row>
     <row r="48" spans="1:2" ht="11" customHeight="1">
       <c r="A48" s="32">
         <v>0.53472222222222399</v>
       </c>
-      <c r="B48" s="91"/>
+      <c r="B48" s="92"/>
     </row>
     <row r="49" spans="1:2" ht="11" customHeight="1">
       <c r="A49" s="32">
         <v>0.53819444444444597</v>
       </c>
-      <c r="B49" s="91"/>
+      <c r="B49" s="92"/>
     </row>
     <row r="50" spans="1:2" ht="11" customHeight="1">
       <c r="A50" s="32">
         <v>0.54166666666666896</v>
       </c>
-      <c r="B50" s="91"/>
+      <c r="B50" s="92"/>
     </row>
     <row r="51" spans="1:2" ht="11" customHeight="1">
       <c r="A51" s="32">
         <v>0.54513888888889095</v>
       </c>
-      <c r="B51" s="91"/>
+      <c r="B51" s="92"/>
     </row>
     <row r="52" spans="1:2" ht="11" customHeight="1">
       <c r="A52" s="32">
         <v>0.54861111111111305</v>
       </c>
-      <c r="B52" s="91"/>
+      <c r="B52" s="92"/>
     </row>
     <row r="53" spans="1:2" ht="11" customHeight="1">
       <c r="A53" s="32">
         <v>0.55208333333333603</v>
       </c>
-      <c r="B53" s="91"/>
+      <c r="B53" s="92"/>
     </row>
     <row r="54" spans="1:2" ht="11" customHeight="1">
       <c r="A54" s="32">
         <v>0.55555555555555802</v>
       </c>
-      <c r="B54" s="91"/>
+      <c r="B54" s="92"/>
     </row>
     <row r="55" spans="1:2" ht="11" customHeight="1">
       <c r="A55" s="32">
         <v>0.55902777777778001</v>
       </c>
-      <c r="B55" s="91"/>
+      <c r="B55" s="92"/>
     </row>
     <row r="56" spans="1:2" ht="11" customHeight="1">
       <c r="A56" s="32">
         <v>0.562500000000002</v>
       </c>
+      <c r="B56" s="93" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="57" spans="1:2" ht="11" customHeight="1">
       <c r="A57" s="32">
         <v>0.56597222222222499</v>
       </c>
+      <c r="B57" s="93"/>
     </row>
     <row r="58" spans="1:2" ht="11" customHeight="1">
       <c r="A58" s="32">
         <v>0.56944444444444697</v>
       </c>
+      <c r="B58" s="90" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="59" spans="1:2" ht="11" customHeight="1">
       <c r="A59" s="32">
         <v>0.57291666666666896</v>
       </c>
+      <c r="B59" s="90"/>
     </row>
     <row r="60" spans="1:2" ht="11" customHeight="1">
       <c r="A60" s="32">
         <v>0.57638888888889095</v>
       </c>
+      <c r="B60" s="90"/>
     </row>
     <row r="61" spans="1:2" ht="11" customHeight="1">
       <c r="A61" s="32">
         <v>0.57986111111111405</v>
       </c>
+      <c r="B61" s="90"/>
     </row>
     <row r="62" spans="1:2" ht="11" customHeight="1">
       <c r="A62" s="32">
         <v>0.58333333333333603</v>
       </c>
+      <c r="B62" s="90"/>
     </row>
     <row r="63" spans="1:2" ht="11" customHeight="1">
       <c r="A63" s="32">
         <v>0.58680555555555802</v>
       </c>
+      <c r="B63" s="90"/>
     </row>
     <row r="64" spans="1:2" ht="11" customHeight="1">
       <c r="A64" s="32">
         <v>0.59027777777778001</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="11" customHeight="1">
+      <c r="B64" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="11" customHeight="1">
       <c r="A65" s="32">
         <v>0.593750000000003</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" ht="11" customHeight="1">
+      <c r="B65" s="35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="11" customHeight="1">
       <c r="A66" s="32">
         <v>0.59722222222222499</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" ht="11" customHeight="1">
+      <c r="B66" s="90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="11" customHeight="1">
       <c r="A67" s="32">
         <v>0.60069444444444697</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" ht="11" customHeight="1">
+      <c r="B67" s="90"/>
+    </row>
+    <row r="68" spans="1:2" ht="11" customHeight="1">
       <c r="A68" s="32">
         <v>0.60416666666666996</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" ht="11" customHeight="1">
+      <c r="B68" s="92" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="11" customHeight="1">
       <c r="A69" s="32">
         <v>0.60763888888889195</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" ht="11" customHeight="1">
+      <c r="B69" s="92"/>
+    </row>
+    <row r="70" spans="1:2" ht="11" customHeight="1">
       <c r="A70" s="32">
         <v>0.61111111111111405</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" ht="11" customHeight="1">
+      <c r="B70" s="92"/>
+    </row>
+    <row r="71" spans="1:2" ht="11" customHeight="1">
       <c r="A71" s="32">
         <v>0.61458333333333603</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" ht="11" customHeight="1">
+      <c r="B71" s="94" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="11" customHeight="1">
       <c r="A72" s="32">
         <v>0.61805555555555902</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" ht="11" customHeight="1">
+      <c r="B72" s="99"/>
+    </row>
+    <row r="73" spans="1:2" ht="11" customHeight="1">
       <c r="A73" s="32">
         <v>0.62152777777778101</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" ht="11" customHeight="1">
+      <c r="B73" s="99"/>
+    </row>
+    <row r="74" spans="1:2" ht="11" customHeight="1">
       <c r="A74" s="32">
         <v>0.625000000000003</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" ht="11" customHeight="1">
+      <c r="B74" s="95"/>
+    </row>
+    <row r="75" spans="1:2" ht="11" customHeight="1">
       <c r="A75" s="32">
         <v>0.62847222222222499</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" ht="11" customHeight="1">
+      <c r="B75" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="11" customHeight="1">
       <c r="A76" s="32">
         <v>0.63194444444444797</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" ht="11" customHeight="1">
+      <c r="B76" s="96" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="11" customHeight="1">
       <c r="A77" s="32">
         <v>0.63541666666666996</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" ht="11" customHeight="1">
+      <c r="B77" s="97"/>
+    </row>
+    <row r="78" spans="1:2" ht="11" customHeight="1">
       <c r="A78" s="32">
         <v>0.63888888888889195</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" ht="11" customHeight="1">
+      <c r="B78" s="94" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="11" customHeight="1">
       <c r="A79" s="32">
         <v>0.64236111111111405</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" ht="11" customHeight="1">
+      <c r="B79" s="99"/>
+    </row>
+    <row r="80" spans="1:2" ht="11" customHeight="1">
       <c r="A80" s="32">
         <v>0.64583333333333703</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" ht="11" customHeight="1">
+      <c r="B80" s="99"/>
+    </row>
+    <row r="81" spans="1:2" ht="11" customHeight="1">
       <c r="A81" s="32">
         <v>0.64930555555555902</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="11" customHeight="1">
+      <c r="B81" s="99"/>
+    </row>
+    <row r="82" spans="1:2" ht="11" customHeight="1">
       <c r="A82" s="32">
         <v>0.65277777777778101</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" ht="11" customHeight="1">
+      <c r="B82" s="99"/>
+    </row>
+    <row r="83" spans="1:2" ht="11" customHeight="1">
       <c r="A83" s="32">
         <v>0.656250000000003</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="11" customHeight="1">
+      <c r="B83" s="95"/>
+    </row>
+    <row r="84" spans="1:2" ht="11" customHeight="1">
       <c r="A84" s="32">
         <v>0.65972222222222598</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" ht="11" customHeight="1">
+      <c r="B84" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="11" customHeight="1">
       <c r="A85" s="32">
         <v>0.66319444444444797</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" ht="11" customHeight="1">
+      <c r="B85" s="96" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="11" customHeight="1">
       <c r="A86" s="32">
         <v>0.66666666666666996</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" ht="11" customHeight="1">
+      <c r="B86" s="97"/>
+    </row>
+    <row r="87" spans="1:2" ht="11" customHeight="1">
       <c r="A87" s="32">
         <v>0.67013888888889295</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" ht="11" customHeight="1">
+      <c r="B87" s="94" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="11" customHeight="1">
       <c r="A88" s="32">
         <v>0.67361111111111505</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" ht="11" customHeight="1">
+      <c r="B88" s="99"/>
+    </row>
+    <row r="89" spans="1:2" ht="11" customHeight="1">
       <c r="A89" s="32">
         <v>0.67708333333333703</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" ht="11" customHeight="1">
+      <c r="B89" s="99"/>
+    </row>
+    <row r="90" spans="1:2" ht="11" customHeight="1">
       <c r="A90" s="32">
         <v>0.68055555555555902</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" ht="11" customHeight="1">
+      <c r="B90" s="99"/>
+    </row>
+    <row r="91" spans="1:2" ht="11" customHeight="1">
       <c r="A91" s="32">
         <v>0.68402777777778201</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" ht="11" customHeight="1">
+      <c r="B91" s="99"/>
+    </row>
+    <row r="92" spans="1:2" ht="11" customHeight="1">
       <c r="A92" s="32">
         <v>0.687500000000004</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" ht="11" customHeight="1">
+      <c r="B92" s="99"/>
+    </row>
+    <row r="93" spans="1:2" ht="11" customHeight="1">
       <c r="A93" s="32">
         <v>0.69097222222222598</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" ht="11" customHeight="1">
+      <c r="B93" s="99"/>
+    </row>
+    <row r="94" spans="1:2" ht="11" customHeight="1">
       <c r="A94" s="32">
         <v>0.69444444444444797</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" ht="11" customHeight="1">
+      <c r="B94" s="99"/>
+    </row>
+    <row r="95" spans="1:2" ht="11" customHeight="1">
       <c r="A95" s="32">
         <v>0.69791666666667096</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" ht="11" customHeight="1">
+      <c r="B95" s="96" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="11" customHeight="1">
       <c r="A96" s="32">
         <v>0.70138888888889295</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" ht="11" customHeight="1">
+      <c r="B96" s="100"/>
+    </row>
+    <row r="97" spans="1:2" ht="11" customHeight="1">
       <c r="A97" s="32">
         <v>0.70486111111111505</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" ht="11" customHeight="1">
+      <c r="B97" s="100"/>
+    </row>
+    <row r="98" spans="1:2" ht="11" customHeight="1">
       <c r="A98" s="32">
         <v>0.70833333333333703</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" ht="11" customHeight="1"/>
-    <row r="100" spans="1:1" ht="11" customHeight="1"/>
-    <row r="101" spans="1:1" ht="11" customHeight="1"/>
-    <row r="102" spans="1:1" ht="11" customHeight="1"/>
+      <c r="B98" s="97"/>
+    </row>
+    <row r="99" spans="1:2" ht="11" customHeight="1"/>
+    <row r="100" spans="1:2" ht="11" customHeight="1"/>
+    <row r="101" spans="1:2" ht="11" customHeight="1"/>
+    <row r="102" spans="1:2" ht="11" customHeight="1"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="B44:B55"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
+  <mergeCells count="22">
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B83"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B94"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B71:B74"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="B44:B55"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="5" scale="79" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>